<commit_message>
Refactor code && edit userlist -> show role
</commit_message>
<xml_diff>
--- a/document/Issues Report.xlsx
+++ b/document/Issues Report.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Documents\SWP\Done\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repositories\Project\g6\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B3E8AC-BE64-40C7-AB1C-0CC132776C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF565E1-2039-4440-8313-6BD9B2DBE25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{1F029D15-4B34-8B4D-AA03-001B4FC8F913}"/>
   </bookViews>
   <sheets>
-    <sheet name="foxz" sheetId="2" state="veryHidden" r:id=""/>
-    <sheet name="Issues Report" sheetId="1" r:id="rId1"/>
+    <sheet name="foxz" sheetId="2" state="veryHidden" r:id="rId1"/>
+    <sheet name="Issues Report" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="149">
   <si>
     <t>Title</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Integrate User Login screen with others</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>Closed</t>
@@ -449,15 +446,6 @@
     <t>3_Done</t>
   </si>
   <si>
-    <t>1_To Do</t>
-  </si>
-  <si>
-    <t>2_Doing</t>
-  </si>
-  <si>
-    <t>2_Doing,Task</t>
-  </si>
-  <si>
     <t>3_Done,Task</t>
   </si>
   <si>
@@ -477,6 +465,42 @@
   </si>
   <si>
     <t>User Profile</t>
+  </si>
+  <si>
+    <t>error handler 404</t>
+  </si>
+  <si>
+    <t>Setup permission system</t>
+  </si>
+  <si>
+    <t>Login with google</t>
+  </si>
+  <si>
+    <t>Intergrate Setting List, Setting Detail and Password Change</t>
+  </si>
+  <si>
+    <t>https://gitlab.com/fu-kiennt-fall22/se1627-net_swp391/g6/-/issues/45</t>
+  </si>
+  <si>
+    <t>iter2</t>
+  </si>
+  <si>
+    <t>https://gitlab.com/fu-kiennt-fall22/se1627-net_swp391/g6/-/issues/46</t>
+  </si>
+  <si>
+    <t>iter3</t>
+  </si>
+  <si>
+    <t>https://gitlab.com/fu-kiennt-fall22/se1627-net_swp391/g6/-/issues/47</t>
+  </si>
+  <si>
+    <t>iter4</t>
+  </si>
+  <si>
+    <t>https://gitlab.com/fu-kiennt-fall22/se1627-net_swp391/g6/-/issues/48</t>
+  </si>
+  <si>
+    <t>iter5</t>
   </si>
 </sst>
 </file>
@@ -612,7 +636,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -637,12 +661,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -963,12 +981,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B9144B-93AC-0243-B48F-1FC49AC75151}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -1023,20 +1053,20 @@
     </row>
     <row r="2" spans="1:11" ht="30.75" thickBot="1">
       <c r="A2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G2" s="8">
         <v>44812.22</v>
@@ -1045,31 +1075,31 @@
         <v>44817.22</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="39.75" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="8">
         <v>44817.287465277775</v>
@@ -1078,31 +1108,31 @@
         <v>44822.287465277775</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="30.75" thickBot="1">
       <c r="A4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G4" s="8">
         <v>44817.299178240741</v>
@@ -1111,31 +1141,31 @@
         <v>44822.299178240741</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="30.75" thickBot="1">
       <c r="A5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="3">
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G5" s="8">
         <v>44817.301030092596</v>
@@ -1144,31 +1174,31 @@
         <v>44822.301030092596</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="30.75" thickBot="1">
       <c r="A6" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G6" s="8">
         <v>44817.303078703706</v>
@@ -1177,33 +1207,33 @@
         <v>44822.303078703706</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30.75" thickBot="1">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="3">
         <v>6</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G7" s="8">
         <v>44817.304201388892</v>
@@ -1212,33 +1242,33 @@
         <v>44822.304201388892</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>131</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30.75" thickBot="1">
       <c r="A8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="3">
         <v>7</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G8" s="8">
         <v>44817.305034722223</v>
@@ -1247,33 +1277,33 @@
         <v>44822.305034722223</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>136</v>
+        <v>129</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="52.5" thickBot="1">
       <c r="A9" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="3">
         <v>8</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G9" s="8">
         <v>44817.307685185187</v>
@@ -1282,33 +1312,33 @@
         <v>44822.307685185187</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="116.25" thickBot="1">
       <c r="A10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="3">
         <v>9</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G10" s="8">
         <v>44817.308564814812</v>
@@ -1317,33 +1347,33 @@
         <v>44822.308564814812</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="65.25" thickBot="1">
       <c r="A11" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="3">
         <v>10</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G11" s="8">
         <v>44817.309560185182</v>
@@ -1352,33 +1382,33 @@
         <v>44822.309560185182</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30.75" thickBot="1">
       <c r="A12" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="3">
         <v>11</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G12" s="8">
         <v>44817.310046296298</v>
@@ -1387,33 +1417,33 @@
         <v>44822.310046296298</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="90.75" thickBot="1">
       <c r="A13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="3">
         <v>12</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G13" s="8">
         <v>44817.310578703706</v>
@@ -1422,33 +1452,33 @@
         <v>44822.310578703706</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30.75" thickBot="1">
       <c r="A14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="3">
         <v>13</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G14" s="8">
         <v>44817.311203703706</v>
@@ -1457,31 +1487,31 @@
         <v>44822.311203703706</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" ht="65.25" thickBot="1">
       <c r="A15" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="3">
         <v>14</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G15" s="8">
         <v>44817.311631944445</v>
@@ -1490,33 +1520,33 @@
         <v>44822.311631944445</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="30.75" thickBot="1">
       <c r="A16" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="3">
         <v>15</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G16" s="8">
         <v>44817.312256944446</v>
@@ -1525,33 +1555,33 @@
         <v>44822.312256944446</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="103.5" thickBot="1">
       <c r="A17" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="3">
         <v>16</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G17" s="8">
         <v>44817.312685185185</v>
@@ -1560,33 +1590,33 @@
         <v>44822.312685185185</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30.75" thickBot="1">
       <c r="A18" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="3">
         <v>17</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G18" s="8">
         <v>44817.313599537039</v>
@@ -1595,33 +1625,33 @@
         <v>44822.313599537039</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="30.75" thickBot="1">
       <c r="A19" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="3">
         <v>18</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G19" s="8">
         <v>44817.314027777778</v>
@@ -1630,33 +1660,33 @@
         <v>44822.314027777778</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="30.75" thickBot="1">
       <c r="A20" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="3">
         <v>19</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G20" s="8">
         <v>44817.314479166664</v>
@@ -1665,13 +1695,13 @@
         <v>44822.314479166664</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30.75" thickBot="1">
@@ -1679,19 +1709,19 @@
         <v>11</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G21" s="8">
         <v>44821.741041666668</v>
@@ -1700,10 +1730,10 @@
         <v>44826.741041666668</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>11</v>
@@ -1715,16 +1745,16 @@
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G22" s="8">
         <v>44821.743148148147</v>
@@ -1733,10 +1763,10 @@
         <v>44826.743148148147</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>11</v>
@@ -1748,16 +1778,16 @@
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G23" s="8">
         <v>44821.743495370371</v>
@@ -1766,10 +1796,10 @@
         <v>44826.743495370371</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>11</v>
@@ -1781,16 +1811,16 @@
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G24" s="8">
         <v>44821.743946759256</v>
@@ -1799,10 +1829,10 @@
         <v>44826.743946759256</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K24" s="6" t="s">
         <v>11</v>
@@ -1814,16 +1844,16 @@
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G25" s="8">
         <v>44821.744409722225</v>
@@ -1832,10 +1862,10 @@
         <v>44826.744409722225</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>11</v>
@@ -1843,20 +1873,20 @@
     </row>
     <row r="26" spans="1:11" ht="39.75" thickBot="1">
       <c r="A26" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G26" s="8">
         <v>44822.098356481481</v>
@@ -1865,29 +1895,29 @@
         <v>44827.098356481481</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" ht="30.75" thickBot="1">
       <c r="A27" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G27" s="8">
         <v>44822.100821759261</v>
@@ -1896,29 +1926,29 @@
         <v>44827.100821759261</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" ht="30.75" thickBot="1">
       <c r="A28" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G28" s="8">
         <v>44822.103032407409</v>
@@ -1927,31 +1957,31 @@
         <v>44827.103032407409</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="30.75" thickBot="1">
       <c r="A29" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G29" s="8">
         <v>44822.103518518517</v>
@@ -1960,31 +1990,31 @@
         <v>44827.103518518517</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="30.75" thickBot="1">
       <c r="A30" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G30" s="8">
         <v>44822.104016203702</v>
@@ -1993,31 +2023,31 @@
         <v>44827.104016203702</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30.75" thickBot="1">
       <c r="A31" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G31" s="8">
         <v>44822.342638888891</v>
@@ -2026,31 +2056,31 @@
         <v>44827.342638888891</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K31" s="3"/>
     </row>
     <row r="32" spans="1:11" ht="39.75" thickBot="1">
       <c r="A32" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C32" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G32" s="8">
         <v>44822.392592592594</v>
@@ -2059,31 +2089,31 @@
         <v>44827.392592592594</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K32" s="3"/>
     </row>
     <row r="33" spans="1:11" ht="30.75" thickBot="1">
       <c r="A33" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G33" s="8">
         <v>44822.399548611109</v>
@@ -2092,29 +2122,29 @@
         <v>44827.399548611109</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K33" s="3"/>
     </row>
     <row r="34" spans="1:11" ht="30.75" thickBot="1">
       <c r="A34" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G34" s="8">
         <v>44822.40902777778</v>
@@ -2123,31 +2153,31 @@
         <v>44827.40902777778</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="30.75" thickBot="1">
       <c r="A35" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G35" s="8">
         <v>44822.409687500003</v>
@@ -2156,31 +2186,31 @@
         <v>44827.409687500003</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="30.75" thickBot="1">
       <c r="A36" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G36" s="8">
         <v>44822.410185185188</v>
@@ -2189,31 +2219,31 @@
         <v>44827.410185185188</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="30.75" thickBot="1">
       <c r="A37" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G37" s="8">
         <v>44822.410671296297</v>
@@ -2222,31 +2252,31 @@
         <v>44827.410671296297</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="30.75" thickBot="1">
       <c r="A38" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G38" s="8">
         <v>44822.411006944443</v>
@@ -2255,31 +2285,31 @@
         <v>44827.411006944443</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="30.75" thickBot="1">
       <c r="A39" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G39" s="8">
         <v>44822.41138888889</v>
@@ -2288,31 +2318,31 @@
         <v>44827.41138888889</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="30.75" thickBot="1">
       <c r="A40" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G40" s="8">
         <v>44822.411874999998</v>
@@ -2321,31 +2351,31 @@
         <v>44827.411874999998</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="30.75" thickBot="1">
       <c r="A41" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G41" s="8">
         <v>44822.412187499998</v>
@@ -2354,31 +2384,31 @@
         <v>44827.412187499998</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="30.75" thickBot="1">
       <c r="A42" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G42" s="8">
         <v>44822.412465277775</v>
@@ -2387,31 +2417,31 @@
         <v>44827.412465277775</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="39.75" thickBot="1">
       <c r="A43" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G43" s="8">
         <v>44822.46329861111</v>
@@ -2420,29 +2450,29 @@
         <v>44827.46329861111</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K43" s="3"/>
     </row>
     <row r="44" spans="1:11" ht="39.75" thickBot="1">
       <c r="A44" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G44" s="8">
         <v>44822.463958333334</v>
@@ -2451,60 +2481,139 @@
         <v>44827.463958333334</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="1:11" ht="30.75" thickBot="1">
+      <c r="A45" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="3">
+        <v>45</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G45" s="8">
+        <v>44822.463958333334</v>
+      </c>
+      <c r="H45" s="4">
+        <v>44827.463958333334</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:11" ht="30.75" thickBot="1">
+      <c r="A46" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="3">
+        <v>46</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G46" s="8">
+        <v>44822.463958333334</v>
+      </c>
+      <c r="H46" s="4">
+        <v>44827.463958333334</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:11" ht="30.75" thickBot="1">
+      <c r="A47" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="3">
+        <v>47</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G47" s="8">
+        <v>44822.463958333334</v>
+      </c>
+      <c r="H47" s="4">
+        <v>44827.463958333334</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="1:11" ht="30.75" thickBot="1">
+      <c r="A48" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" s="6"/>
+      <c r="C48" s="3">
+        <v>48</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G48" s="8">
+        <v>44822.463958333334</v>
+      </c>
+      <c r="H48" s="4">
+        <v>44827.463958333334</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K48" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{2208D63C-48EF-4DD2-BDEE-7D973591A74A}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{EA5762CD-CEE1-4652-8771-647A5A4C15A8}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{FF311DE9-DD4A-464E-8A2F-068826DB7B60}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{990DB32B-6158-49C0-ADC4-479C59A75829}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{A0FEF0FD-ACFC-4C07-8B90-7D4879955F9D}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{99006478-BDE0-4CD5-B4AA-E53C8FBC2D5C}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{1AA55E40-E07B-4BA0-86C4-D444717AE5F7}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{183BC535-350D-4420-B7DE-4A671B0F4A50}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{8690F510-4A0E-434A-8F3D-CEA552865E2B}"/>
-    <hyperlink ref="D11" r:id="rId10" xr:uid="{AF0BDB6C-C553-4214-899B-6DAE0CC2A428}"/>
-    <hyperlink ref="D12" r:id="rId11" xr:uid="{FFEFB05E-E8F4-4CE7-9DF9-D5287BD6925E}"/>
-    <hyperlink ref="D13" r:id="rId12" xr:uid="{A5606261-2BF0-4FBF-B333-8A22F327FF9B}"/>
-    <hyperlink ref="D14" r:id="rId13" xr:uid="{E192321D-1659-459B-A5D0-1194AB8F2A25}"/>
-    <hyperlink ref="D15" r:id="rId14" xr:uid="{09ECF8E4-06D9-42F0-BCDA-D73336FB1DF9}"/>
-    <hyperlink ref="D16" r:id="rId15" xr:uid="{805A766F-A0A0-423A-9D87-D563CD5A16C4}"/>
-    <hyperlink ref="D17" r:id="rId16" xr:uid="{07398AE4-8375-424F-97F4-70BF4829731A}"/>
-    <hyperlink ref="D18" r:id="rId17" xr:uid="{B65E1FC6-5BD6-4663-8A50-6D8376809751}"/>
-    <hyperlink ref="D19" r:id="rId18" xr:uid="{EBB3883F-7923-47D0-BA84-6177E2D65896}"/>
-    <hyperlink ref="D20" r:id="rId19" xr:uid="{07D4F219-C2C2-4E79-94C8-1397C19EF73D}"/>
-    <hyperlink ref="D21" r:id="rId20" xr:uid="{11D03E82-993A-4288-80BB-D118BFFDEC01}"/>
-    <hyperlink ref="D22" r:id="rId21" xr:uid="{890542E6-6441-409C-9C20-35106916F88D}"/>
-    <hyperlink ref="D23" r:id="rId22" xr:uid="{A886A906-6169-4934-BA00-D4F03333A188}"/>
-    <hyperlink ref="D24" r:id="rId23" xr:uid="{3ADA0AFA-C1B9-40F7-B16E-55FB72DAF244}"/>
-    <hyperlink ref="D25" r:id="rId24" xr:uid="{8D8A5D83-5447-4865-9EE5-BCA1A0C3FC04}"/>
-    <hyperlink ref="D26" r:id="rId25" xr:uid="{B5DC0A9B-40A5-4CFE-9108-943878187CDE}"/>
-    <hyperlink ref="D27" r:id="rId26" xr:uid="{06720E45-7FFF-4A0D-8595-C53B7A11C472}"/>
-    <hyperlink ref="D28" r:id="rId27" xr:uid="{C1C53371-908E-4DF7-A81B-798AE425B1DF}"/>
-    <hyperlink ref="D29" r:id="rId28" xr:uid="{D811317E-431A-45CA-89A5-4A9E2E74D68B}"/>
-    <hyperlink ref="D30" r:id="rId29" xr:uid="{F6645CDB-BF03-42CE-A2C6-2A4C6472FE67}"/>
-    <hyperlink ref="D31" r:id="rId30" xr:uid="{7340722A-0A87-4F90-8DE1-2FB76A50D182}"/>
-    <hyperlink ref="D32" r:id="rId31" xr:uid="{9E218AE7-A333-403A-B377-0DDD76934155}"/>
-    <hyperlink ref="D33" r:id="rId32" xr:uid="{29972BE0-FDA1-4EFC-8F1D-454164C108B9}"/>
-    <hyperlink ref="D34" r:id="rId33" xr:uid="{259A261A-20F7-4EEC-9787-8985765A6D6D}"/>
-    <hyperlink ref="D35" r:id="rId34" xr:uid="{15F3E094-4091-48D4-B7DF-E67893B723AE}"/>
-    <hyperlink ref="D36" r:id="rId35" xr:uid="{D0703F15-226C-45CE-B8C1-64A9A0390E81}"/>
-    <hyperlink ref="D37" r:id="rId36" xr:uid="{ED13AFD8-8095-46A3-8F9C-B944D88546C5}"/>
-    <hyperlink ref="D38" r:id="rId37" xr:uid="{C70AE640-72AA-4F53-9D3C-AC194E2CEBD3}"/>
-    <hyperlink ref="D39" r:id="rId38" xr:uid="{F816AB89-BB74-45E5-9750-24B1D9190379}"/>
-    <hyperlink ref="D40" r:id="rId39" xr:uid="{0B954CC8-CABD-4352-AD38-F667A58B204B}"/>
-    <hyperlink ref="D41" r:id="rId40" xr:uid="{67757326-5D69-4365-B78B-F85672782E58}"/>
-    <hyperlink ref="D42" r:id="rId41" xr:uid="{A16C2AD6-BC75-495C-959E-3FC858EA0490}"/>
-    <hyperlink ref="D43" r:id="rId42" xr:uid="{F219D96C-723F-4144-9F73-B66AE60103E0}"/>
-    <hyperlink ref="D44" r:id="rId43" xr:uid="{32F1F048-0A35-4854-BD3C-18C859F6CAE6}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>